<commit_message>
add MS to context related identifier 4e6dc05c306dd93bff0e7c96caa00728b9af086c
</commit_message>
<xml_diff>
--- a/ig/nr-add-ReferenceIdList/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/ig/nr-add-ReferenceIdList/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-02T16:08:22+00:00</t>
+    <t>2023-10-02T16:24:37+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -12958,7 +12958,7 @@
         <v>50</v>
       </c>
       <c r="H81" t="s" s="2">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I81" t="s" s="2">
         <v>35</v>

</xml_diff>

<commit_message>
add MS to context related identifier 53ae3acbe828dd4529bc27d3e5a9c9779405e599
</commit_message>
<xml_diff>
--- a/ig/nr-add-ReferenceIdList/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/ig/nr-add-ReferenceIdList/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-02T16:24:37+00:00</t>
+    <t>2023-10-02T16:25:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -14508,7 +14508,7 @@
         <v>50</v>
       </c>
       <c r="H93" t="s" s="2">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I93" t="s" s="2">
         <v>35</v>
@@ -15032,7 +15032,7 @@
         <v>50</v>
       </c>
       <c r="H97" t="s" s="2">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I97" t="s" s="2">
         <v>35</v>
@@ -15163,7 +15163,7 @@
         <v>50</v>
       </c>
       <c r="H98" t="s" s="2">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I98" t="s" s="2">
         <v>35</v>

</xml_diff>

<commit_message>
update system urn:ietf:rfc:3986 0c3ed428e8aff672c6d669b769a6eb69b4824e68
</commit_message>
<xml_diff>
--- a/ig/nr-add-ReferenceIdList/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/ig/nr-add-ReferenceIdList/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-10T15:16:16+00:00</t>
+    <t>2023-10-10T16:49:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2024,7 +2024,7 @@
     <t>Need to be unambiguous about the source of the definition of the symbol.</t>
   </si>
   <si>
-    <t>ISO</t>
+    <t>urn:ietf:rfc:3986</t>
   </si>
   <si>
     <t>Coding.system</t>

</xml_diff>